<commit_message>
added Judgment games to the yakuza tab & chart
</commit_message>
<xml_diff>
--- a/playstation/output/dates_&_finances_all-time.xlsx
+++ b/playstation/output/dates_&_finances_all-time.xlsx
@@ -33,7 +33,7 @@
     <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">gifts!$A$1:$G$186</definedName>
     <definedName hidden="1" localSheetId="4" name="_xlnm._FilterDatabase">t10hours!$A$1:$H$11</definedName>
     <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">t10value!$A$1:$H$11</definedName>
-    <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">yakuza!$A$1:$H$14</definedName>
+    <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">yakuza!$A$1:$H$16</definedName>
     <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'2025'!$A$1:$G$4</definedName>
     <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">'2024'!$A$1:$G$53</definedName>
     <definedName hidden="1" localSheetId="10" name="_xlnm._FilterDatabase">'2023'!$A$1:$G$84</definedName>
@@ -55,14 +55,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId29" roundtripDataChecksum="ci5PLz3K/jJ/uPGAHmfcaYE5I0bWRdsg/JPZoNGV3ek="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId29" roundtripDataChecksum="tpZUdUFhFB2LPZ5cTRXAb8Ex6Rkwj+6nWvBwW6I/kOI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2875" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2879" uniqueCount="1140">
   <si>
     <t>Tasks</t>
   </si>
@@ -865,6 +865,12 @@
     <t>Playstation Plus Essential Subscription Service</t>
   </si>
   <si>
+    <t>Judgment</t>
+  </si>
+  <si>
+    <t>Lost Judgment</t>
+  </si>
+  <si>
     <t>TY The Tasmanian Tiger 2: Bush Rescue</t>
   </si>
   <si>
@@ -955,9 +961,6 @@
     <t>Empire of Sin</t>
   </si>
   <si>
-    <t>Judgment</t>
-  </si>
-  <si>
     <t>Shadow of the Tomb Raider</t>
   </si>
   <si>
@@ -1052,9 +1055,6 @@
   </si>
   <si>
     <t>Holy Potatoes! What the Hell?!</t>
-  </si>
-  <si>
-    <t>Lost Judgment</t>
   </si>
   <si>
     <t>PowerWash Simulator</t>
@@ -4150,11 +4150,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1149456410"/>
-        <c:axId val="1348902222"/>
+        <c:axId val="951188111"/>
+        <c:axId val="1530657967"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1149456410"/>
+        <c:axId val="951188111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4206,10 +4206,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1348902222"/>
+        <c:crossAx val="1530657967"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1348902222"/>
+        <c:axId val="1530657967"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4284,7 +4284,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1149456410"/>
+        <c:crossAx val="951188111"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
@@ -4381,11 +4381,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2032950242"/>
-        <c:axId val="1957747848"/>
+        <c:axId val="1485541669"/>
+        <c:axId val="2050143369"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2032950242"/>
+        <c:axId val="1485541669"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4437,10 +4437,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1957747848"/>
+        <c:crossAx val="2050143369"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1957747848"/>
+        <c:axId val="2050143369"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4515,7 +4515,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2032950242"/>
+        <c:crossAx val="1485541669"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -4618,11 +4618,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="384264720"/>
-        <c:axId val="23887375"/>
+        <c:axId val="884792572"/>
+        <c:axId val="458139188"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="384264720"/>
+        <c:axId val="884792572"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4674,10 +4674,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23887375"/>
+        <c:crossAx val="458139188"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23887375"/>
+        <c:axId val="458139188"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4752,7 +4752,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384264720"/>
+        <c:crossAx val="884792572"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -4859,21 +4859,21 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>yakuza!$B$2:$B$39</c:f>
+              <c:f>yakuza!$B$2:$B$41</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>yakuza!$G$2:$G$39</c:f>
+              <c:f>yakuza!$G$2:$G$41</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="555583061"/>
-        <c:axId val="195625712"/>
+        <c:axId val="1024431974"/>
+        <c:axId val="1358650772"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="555583061"/>
+        <c:axId val="1024431974"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4925,10 +4925,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195625712"/>
+        <c:crossAx val="1358650772"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195625712"/>
+        <c:axId val="1358650772"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5003,7 +5003,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="555583061"/>
+        <c:crossAx val="1024431974"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -5145,11 +5145,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1877634631"/>
-        <c:axId val="1223169642"/>
+        <c:axId val="1745961001"/>
+        <c:axId val="577518907"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1877634631"/>
+        <c:axId val="1745961001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5201,10 +5201,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1223169642"/>
+        <c:crossAx val="577518907"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1223169642"/>
+        <c:axId val="577518907"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5279,7 +5279,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1877634631"/>
+        <c:crossAx val="1745961001"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -5494,7 +5494,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7305675" cy="4505325"/>
@@ -7772,7 +7772,7 @@
         <v>830.0</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C6" s="111" t="s">
         <v>36</v>
@@ -7796,7 +7796,7 @@
         <v>1030.0</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C7" s="111" t="s">
         <v>49</v>
@@ -7868,7 +7868,7 @@
         <v>1021.0</v>
       </c>
       <c r="B10" s="105" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C10" s="111" t="s">
         <v>49</v>
@@ -7892,7 +7892,7 @@
         <v>592.0</v>
       </c>
       <c r="B11" s="105" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C11" s="111" t="s">
         <v>36</v>
@@ -8011,7 +8011,7 @@
         <v>295.0</v>
       </c>
       <c r="B16" s="111" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C16" s="111" t="s">
         <v>31</v>
@@ -8034,7 +8034,7 @@
         <v>1027.0</v>
       </c>
       <c r="B17" s="111" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C17" s="111" t="s">
         <v>49</v>
@@ -8082,7 +8082,7 @@
         <v>520.0</v>
       </c>
       <c r="B19" s="111" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C19" s="111" t="s">
         <v>36</v>
@@ -8106,7 +8106,7 @@
         <v>924.0</v>
       </c>
       <c r="B20" s="111" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C20" s="111" t="s">
         <v>36</v>
@@ -8130,7 +8130,7 @@
         <v>1026.0</v>
       </c>
       <c r="B21" s="111" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C21" s="111" t="s">
         <v>49</v>
@@ -8154,7 +8154,7 @@
         <v>567.0</v>
       </c>
       <c r="B22" s="111" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C22" s="111" t="s">
         <v>36</v>
@@ -8178,7 +8178,7 @@
         <v>594.0</v>
       </c>
       <c r="B23" s="111" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C23" s="111" t="s">
         <v>36</v>
@@ -8202,7 +8202,7 @@
         <v>768.0</v>
       </c>
       <c r="B24" s="111" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C24" s="111" t="s">
         <v>36</v>
@@ -8274,7 +8274,7 @@
         <v>586.0</v>
       </c>
       <c r="B27" s="111" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C27" s="111" t="s">
         <v>36</v>
@@ -8298,7 +8298,7 @@
         <v>1017.0</v>
       </c>
       <c r="B28" s="111" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C28" s="111" t="s">
         <v>49</v>
@@ -8490,7 +8490,7 @@
         <v>1035.0</v>
       </c>
       <c r="B36" s="111" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C36" s="111" t="s">
         <v>89</v>
@@ -8562,7 +8562,7 @@
         <v>1037.0</v>
       </c>
       <c r="B39" s="116" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C39" s="115" t="s">
         <v>49</v>
@@ -8586,7 +8586,7 @@
         <v>1038.0</v>
       </c>
       <c r="B40" s="116" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C40" s="115" t="s">
         <v>36</v>
@@ -8610,7 +8610,7 @@
         <v>1039.0</v>
       </c>
       <c r="B41" s="116" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C41" s="115" t="s">
         <v>99</v>
@@ -8634,7 +8634,7 @@
         <v>1040.0</v>
       </c>
       <c r="B42" s="116" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C42" s="115" t="s">
         <v>99</v>
@@ -8658,7 +8658,7 @@
         <v>1041.0</v>
       </c>
       <c r="B43" s="116" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C43" s="115" t="s">
         <v>99</v>
@@ -8730,7 +8730,7 @@
         <v>1044.0</v>
       </c>
       <c r="B46" s="116" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C46" s="116" t="s">
         <v>49</v>
@@ -8754,7 +8754,7 @@
         <v>1045.0</v>
       </c>
       <c r="B47" s="56" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C47" s="116" t="s">
         <v>49</v>
@@ -8778,7 +8778,7 @@
         <v>1046.0</v>
       </c>
       <c r="B48" s="116" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C48" s="116" t="s">
         <v>49</v>
@@ -8802,7 +8802,7 @@
         <v>1047.0</v>
       </c>
       <c r="B49" s="116" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C49" s="116" t="s">
         <v>49</v>
@@ -9052,7 +9052,7 @@
         <v>881.0</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C3" s="111" t="s">
         <v>36</v>
@@ -9075,7 +9075,7 @@
         <v>895.0</v>
       </c>
       <c r="B4" s="111" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C4" s="111" t="s">
         <v>36</v>
@@ -9145,7 +9145,7 @@
         <v>771.0</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C7" s="111" t="s">
         <v>36</v>
@@ -9168,7 +9168,7 @@
         <v>595.0</v>
       </c>
       <c r="B8" s="111" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C8" s="111" t="s">
         <v>36</v>
@@ -9237,7 +9237,7 @@
         <v>667.0</v>
       </c>
       <c r="B11" s="105" t="s">
-        <v>297</v>
+        <v>267</v>
       </c>
       <c r="C11" s="111" t="s">
         <v>36</v>
@@ -9352,7 +9352,7 @@
         <v>812.0</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C16" s="111" t="s">
         <v>36</v>
@@ -9467,7 +9467,7 @@
         <v>175.0</v>
       </c>
       <c r="B21" s="105" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C21" s="111" t="s">
         <v>31</v>
@@ -9490,7 +9490,7 @@
         <v>583.0</v>
       </c>
       <c r="B22" s="105" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C22" s="111" t="s">
         <v>36</v>
@@ -9513,7 +9513,7 @@
         <v>635.0</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C23" s="111" t="s">
         <v>36</v>
@@ -9536,7 +9536,7 @@
         <v>969.0</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C24" s="111" t="s">
         <v>109</v>
@@ -9582,7 +9582,7 @@
         <v>909.0</v>
       </c>
       <c r="B26" s="105" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C26" s="111" t="s">
         <v>36</v>
@@ -9605,7 +9605,7 @@
         <v>927.0</v>
       </c>
       <c r="B27" s="105" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C27" s="111" t="s">
         <v>36</v>
@@ -9628,7 +9628,7 @@
         <v>928.0</v>
       </c>
       <c r="B28" s="105" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C28" s="111" t="s">
         <v>36</v>
@@ -9651,7 +9651,7 @@
         <v>929.0</v>
       </c>
       <c r="B29" s="105" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C29" s="111" t="s">
         <v>36</v>
@@ -9674,7 +9674,7 @@
         <v>748.0</v>
       </c>
       <c r="B30" s="105" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C30" s="111" t="s">
         <v>36</v>
@@ -9697,7 +9697,7 @@
         <v>415.0</v>
       </c>
       <c r="B31" s="105" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C31" s="111" t="s">
         <v>31</v>
@@ -9720,7 +9720,7 @@
         <v>527.0</v>
       </c>
       <c r="B32" s="105" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C32" s="111" t="s">
         <v>36</v>
@@ -9743,7 +9743,7 @@
         <v>618.0</v>
       </c>
       <c r="B33" s="105" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C33" s="111" t="s">
         <v>36</v>
@@ -9766,7 +9766,7 @@
         <v>858.0</v>
       </c>
       <c r="B34" s="105" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C34" s="111" t="s">
         <v>36</v>
@@ -9858,7 +9858,7 @@
         <v>643.0</v>
       </c>
       <c r="B38" s="111" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C38" s="111" t="s">
         <v>36</v>
@@ -9881,7 +9881,7 @@
         <v>579.0</v>
       </c>
       <c r="B39" s="111" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C39" s="111" t="s">
         <v>36</v>
@@ -9905,7 +9905,7 @@
         <v>276.0</v>
       </c>
       <c r="B40" s="111" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C40" s="111" t="s">
         <v>31</v>
@@ -9998,7 +9998,7 @@
         <v>570.0</v>
       </c>
       <c r="B44" s="105" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C44" s="111" t="s">
         <v>36</v>
@@ -10021,7 +10021,7 @@
         <v>911.0</v>
       </c>
       <c r="B45" s="105" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C45" s="111" t="s">
         <v>36</v>
@@ -10343,7 +10343,7 @@
         <v>930.0</v>
       </c>
       <c r="B59" s="105" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C59" s="111" t="s">
         <v>36</v>
@@ -10412,7 +10412,7 @@
         <v>756.0</v>
       </c>
       <c r="B62" s="105" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C62" s="111" t="s">
         <v>36</v>
@@ -10458,7 +10458,7 @@
         <v>790.0</v>
       </c>
       <c r="B64" s="105" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C64" s="111" t="s">
         <v>36</v>
@@ -10550,7 +10550,7 @@
         <v>1013.0</v>
       </c>
       <c r="B68" s="105" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C68" s="111" t="s">
         <v>49</v>
@@ -10573,7 +10573,7 @@
         <v>1025.0</v>
       </c>
       <c r="B69" s="111" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C69" s="111" t="s">
         <v>49</v>
@@ -10596,7 +10596,7 @@
         <v>130.0</v>
       </c>
       <c r="B70" s="105" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C70" s="111" t="s">
         <v>99</v>
@@ -10642,7 +10642,7 @@
         <v>529.0</v>
       </c>
       <c r="B72" s="105" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C72" s="111" t="s">
         <v>36</v>
@@ -10665,7 +10665,7 @@
         <v>545.0</v>
       </c>
       <c r="B73" s="105" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C73" s="111" t="s">
         <v>36</v>
@@ -10688,7 +10688,7 @@
         <v>546.0</v>
       </c>
       <c r="B74" s="105" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C74" s="111" t="s">
         <v>36</v>
@@ -10711,7 +10711,7 @@
         <v>564.0</v>
       </c>
       <c r="B75" s="105" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C75" s="111" t="s">
         <v>36</v>
@@ -10734,7 +10734,7 @@
         <v>649.0</v>
       </c>
       <c r="B76" s="105" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C76" s="111" t="s">
         <v>36</v>
@@ -10757,7 +10757,7 @@
         <v>650.0</v>
       </c>
       <c r="B77" s="105" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C77" s="111" t="s">
         <v>36</v>
@@ -10780,7 +10780,7 @@
         <v>651.0</v>
       </c>
       <c r="B78" s="105" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C78" s="111" t="s">
         <v>36</v>
@@ -10803,7 +10803,7 @@
         <v>699.0</v>
       </c>
       <c r="B79" s="111" t="s">
-        <v>330</v>
+        <v>268</v>
       </c>
       <c r="C79" s="111" t="s">
         <v>36</v>
@@ -41434,7 +41434,7 @@
         <v>198.0</v>
       </c>
       <c r="H2" s="37">
-        <f t="shared" ref="H2:H14" si="1">E2/G2</f>
+        <f t="shared" ref="H2:H16" si="1">E2/G2</f>
         <v>0.0454040404</v>
       </c>
     </row>
@@ -41602,118 +41602,118 @@
     </row>
     <row r="9">
       <c r="A9" s="14">
-        <v>418.0</v>
+        <v>667.0</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>66</v>
+        <v>267</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D9" s="37">
-        <v>19.99</v>
+        <v>39.99</v>
       </c>
       <c r="E9" s="37">
-        <v>0.0</v>
+        <v>15.97</v>
       </c>
       <c r="F9" s="37">
-        <v>19.99</v>
+        <v>24.02</v>
       </c>
       <c r="G9" s="14">
-        <v>50.0</v>
+        <v>63.0</v>
       </c>
       <c r="H9" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.2534920635</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="14">
-        <v>695.0</v>
+        <v>699.0</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>67</v>
+        <v>268</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="37">
-        <v>54.99</v>
+        <v>89.99</v>
       </c>
       <c r="E10" s="37">
-        <v>0.0</v>
+        <v>22.49</v>
       </c>
       <c r="F10" s="37">
-        <v>54.99</v>
+        <v>67.5</v>
       </c>
       <c r="G10" s="14">
-        <v>47.0</v>
+        <v>52.0</v>
       </c>
       <c r="H10" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.4325</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="14">
-        <v>278.0</v>
+        <v>418.0</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="37">
-        <v>13.33</v>
+        <v>19.99</v>
       </c>
       <c r="E11" s="37">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="F11" s="37">
-        <v>5.33</v>
+        <v>19.99</v>
       </c>
       <c r="G11" s="14">
-        <v>45.0</v>
+        <v>50.0</v>
       </c>
       <c r="H11" s="37">
         <f t="shared" si="1"/>
-        <v>0.1777777778</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="14">
-        <v>693.0</v>
+        <v>695.0</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="37">
-        <v>19.99</v>
+        <v>54.99</v>
       </c>
       <c r="E12" s="37">
-        <v>8.99</v>
+        <v>0.0</v>
       </c>
       <c r="F12" s="37">
-        <v>11.0</v>
+        <v>54.99</v>
       </c>
       <c r="G12" s="14">
-        <v>42.0</v>
+        <v>47.0</v>
       </c>
       <c r="H12" s="37">
         <f t="shared" si="1"/>
-        <v>0.214047619</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="14">
-        <v>279.0</v>
+        <v>278.0</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>31</v>
@@ -41728,45 +41728,99 @@
         <v>5.33</v>
       </c>
       <c r="G13" s="14">
+        <v>45.0</v>
+      </c>
+      <c r="H13" s="37">
+        <f t="shared" si="1"/>
+        <v>0.1777777778</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="14">
+        <v>693.0</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="37">
+        <v>19.99</v>
+      </c>
+      <c r="E14" s="37">
+        <v>8.99</v>
+      </c>
+      <c r="F14" s="37">
+        <v>11.0</v>
+      </c>
+      <c r="G14" s="14">
+        <v>42.0</v>
+      </c>
+      <c r="H14" s="37">
+        <f t="shared" si="1"/>
+        <v>0.214047619</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="14">
+        <v>279.0</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="37">
+        <v>13.33</v>
+      </c>
+      <c r="E15" s="37">
+        <v>8.0</v>
+      </c>
+      <c r="F15" s="37">
+        <v>5.33</v>
+      </c>
+      <c r="G15" s="14">
         <v>38.0</v>
       </c>
-      <c r="H13" s="37">
+      <c r="H15" s="37">
         <f t="shared" si="1"/>
         <v>0.2105263158</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="38">
+    <row r="16">
+      <c r="A16" s="38">
         <v>1051.0</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B16" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C16" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D16" s="21">
         <v>59.99</v>
       </c>
-      <c r="E14" s="21">
-        <v>0.0</v>
-      </c>
-      <c r="F14" s="21">
-        <f>D14-E14</f>
+      <c r="E16" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="F16" s="21">
+        <f>D16-E16</f>
         <v>59.99</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G16" s="14">
         <v>1.0</v>
       </c>
-      <c r="H14" s="37">
+      <c r="H16" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$H$14">
-    <sortState ref="A1:H14">
-      <sortCondition descending="1" ref="G1:G14"/>
+  <autoFilter ref="$A$1:$H$16">
+    <sortState ref="A1:H16">
+      <sortCondition descending="1" ref="G1:G16"/>
     </sortState>
   </autoFilter>
   <drawing r:id="rId1"/>
@@ -42007,7 +42061,7 @@
         <v>1052.0</v>
       </c>
       <c r="B2" s="94" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C2" s="95" t="s">
         <v>99</v>
@@ -42031,7 +42085,7 @@
         <v>1053.0</v>
       </c>
       <c r="B3" s="98" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C3" s="99" t="s">
         <v>36</v>

</xml_diff>